<commit_message>
Final component list with mostly exact component counts
</commit_message>
<xml_diff>
--- a/componentList.xlsx
+++ b/componentList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arda\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arda KASIM\Documents\ELE713-Two-Switch-Flyback\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB2ED6E-59E2-486B-84F7-87BED2122717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACAF1F7-2771-438B-A4B2-2B17C5DF6BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E213F54F-53EC-4B42-AEC9-6F6BEC0714C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="173">
   <si>
     <t>Part Number</t>
   </si>
@@ -512,34 +512,49 @@
     <t>Res: 10 Ω 1 W 1206 0.1%</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/filter/common-mode-chokes/839?s=N4IgjCBcoEwdIDGUBmBDANgZwKYBoQB7KAbRAGYAOAThhnJAF0CAHAFyhAGU2AnASwB2AcxABfAmGqUooZJHTZ8RUuDjkYANiasOkbnyGiJa6gwTzFuAsUhkYlAOybyjkAU3VNMau5CUAVkoAFjcCalCgvzAABhjNRwhJAMcfJPBNYICAhklM6XSwShhUsPBqMC0Y6LM4bQI4Z1i-OjAAmJgW13JQloDNME0AlsdyMeqGyiHNepAfGOlgnRB2Th4BEXFJWnM5VExrFTtwYJgY4N9JYO8wQtDBsra212ig8hdXkPPogYXLjPIbU6eRyYCWkkoPTM0UolEGMm2VDONUyjgR5XywLmMTA5GoZTgwTx4LmrkcRK6jkc2T6M1uLU0MQCRQZYNxrOCbRG73pzBWegMG2M2xosiQ%2ByUNlU1UYJgAtJ0LFA%2BABXZS2MjDWUEOXwPYKA7q1R43yykyKsiIAAWhAA1jhltoEPwACacXU4vyrfR%2BNgATxYDv0aCwyDEYiAA</t>
-  </si>
-  <si>
-    <t>FIND INPUT CHOKE -&gt;</t>
-  </si>
-  <si>
-    <t>FIND INPUT CAP -&gt;</t>
-  </si>
-  <si>
-    <t>FIND OUTPUT CAP -&gt;</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/kemet/R60IN43305030J/12178362</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/R60DN5100AA30J/13176154</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/filter/aluminum-electrolytic-capacitors/58?s=N4IgjCBcoEwAwHYCcVQGMoDMCGAbAzgKYA0IA9lANrhxwAEAaiKWGPUy-I8%2BDAKzcWfdjzAA2ESzECO4BDNEAOSSHgqYbQaq6yY-LTADM64QYkHlW4yIC6pAA4AXKCACqAOwCWjgPKYAsoTY%2BACuAE6EIAC%2BMUA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/filter/ceramic-capacitors/60?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbRADYBOcgJkpALAAYnyB2CR2JgDlh4bgArGzqdhbAMxgagsDxqi2chT14rJNckzmVNYcoJphJPKkbCUeQyUeNCmsgjUlTYy568nlDBWO-J-I20mWF8QLRobHWc2a3cjOKFYegJyHlN4AF0CAAcAFygQAGV8gCcASwA7AHMQAF9nUPpoEGRIdGx8IlIKHgACAFaAMTkh0cYAOhpxuUmhWamBkaNFiOm1mkm2Ncldyb2Vv221oUnyNfJzy8nliZAeDaPwJjWZN9g3heeaGef3WY5EAFIoAVSqFXyAHkUABZHBoLAAVzKOAaBAAtBBWu1OrgCMRIGRJJRUiB3AI-JQYuBFOEwBwnCApEzRDoso0QBjZDioOUkd1CWQhCAOZzDK0KgATIpYpjiEGQECCfIAT1yaKViOQ9XqQA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/filter/ceramic-capacitors/60?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbXAFYBOAJlgHYQCxLYAOWeA6gZlbt8YhqANgAMw8hC59h3BgWGVh1SoLij2rNeToqpQ6mHKjqgnv3ogAugQAOAFyggAyvYBOASwB2AcxABfLlFYVWgQZEh0bHwiUgNRAAIAVoAxNWS0pgA6agy1LNg87PIi8CzWUtzUsxzKrLpS7kaspuqCbizKUth60pK2kHIs4VLhYdHy0ros-syQVlqBygLSsESBsCq5uFXZtQaB6nW56i2zA7nuY8FuVsuugfo%2B64UKgdYzplFrmxAHJwAql4PPYAPIoACyODQWAArm4cAECABaCBhCJRXAEYiQMjcSiqAj0LREyiiNTUOjCfabQT8UwEXTkqyBEDI0zoqDuWExHFkcjWfys6lhDwAEycqNE%2Bn%2BkBAgnsAE9bIi5TDkEKgA</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/filter/aluminum-electrolytic-capacitors/58?s=N4IgjCBcpgnAHLKoDGUBmBDANgZwKYA0IA9lANogAMIAugL7EBMVA7EtCGpFnkaRRBMArAAIAaiGbwJUkAGYqs4vLGTiAFiXqQGpst1q5w7caPFhANgOXTxS-JvmQrOy7AHWz%2BG9i-nYFRuYIEGYCxhImEmYbaxAV5hPgYsbkyhOkwRmVGZiikxmXGZyTqKprTEAA4ALlAgAKoAdgCWNQDy6ACy%2BJi4AK4ATvggjCAAtEzIXFA1g-38ZJCUwnT060A</t>
+    <t>https://www.digikey.com/en/products/detail/kemet/SC-18-10J/10441828</t>
+  </si>
+  <si>
+    <t>Input Choke</t>
+  </si>
+  <si>
+    <t>SC-18-10J</t>
+  </si>
+  <si>
+    <t>R60IN43305030J</t>
+  </si>
+  <si>
+    <t>Input Film Cap</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/R66DD4220AA6AJ/13176308</t>
+  </si>
+  <si>
+    <t>Output Film Cap</t>
+  </si>
+  <si>
+    <t>R66DD4220AA6AJ</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/A768KS227M1VLAE024/12704040</t>
+  </si>
+  <si>
+    <t>Input AlPo Cap</t>
+  </si>
+  <si>
+    <t>A768KS227M1VLAE024</t>
+  </si>
+  <si>
+    <t>Output AlPo Cap</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/A759MS226M2AAAE045/6196528</t>
+  </si>
+  <si>
+    <t>A759MS226M2AAAE045</t>
   </si>
 </sst>
 </file>
@@ -675,7 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -701,12 +716,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -723,7 +737,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1041,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248413FF-8C01-4D2A-8D21-504DC00DAF5E}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,7 +1345,7 @@
       <c r="C19" s="8">
         <v>2</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1345,7 +1359,7 @@
       <c r="C20" s="8">
         <v>3</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1783,146 +1797,200 @@
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+    <row r="52" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C52" s="14">
-        <v>1</v>
-      </c>
-      <c r="D52" s="14" t="s">
+      <c r="C52" s="13">
+        <v>1</v>
+      </c>
+      <c r="D52" s="13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+    <row r="53" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="13">
         <v>2</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
+    <row r="54" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="13">
         <v>2</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
+    <row r="55" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C55" s="14">
-        <v>1</v>
-      </c>
-      <c r="D55" s="15" t="s">
+      <c r="C55" s="13">
+        <v>1</v>
+      </c>
+      <c r="D55" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
+    <row r="56" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="13">
         <v>2</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
+    <row r="57" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="13">
         <v>2</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="13" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
+    <row r="58" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="14">
+      <c r="C58" s="13">
         <v>2</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="14" t="s">
+    <row r="59" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="13">
+        <v>2</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D59" s="13" t="s">
+    </row>
+    <row r="60" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" s="13">
+        <v>2</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C61" s="13">
+        <v>2</v>
+      </c>
+      <c r="D61" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="D60" s="13" t="s">
+    <row r="62" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" s="13">
+        <v>4</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="13">
+        <v>2</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="13">
+        <v>2</v>
+      </c>
+      <c r="D64" s="14" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D63" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="13" t="s">
-        <v>166</v>
+    <row r="65" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="13">
+        <v>4</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1954,10 +2022,10 @@
     <hyperlink ref="D27" r:id="rId25" xr:uid="{C83578F1-EC42-4BE7-A143-53F6DB372D08}"/>
     <hyperlink ref="D56" r:id="rId26" xr:uid="{696FF0EA-0FE5-42FF-90DE-163CFC428437}"/>
     <hyperlink ref="D58" r:id="rId27" xr:uid="{0D6516E8-7CC1-4663-87D0-C1E538F2B339}"/>
-    <hyperlink ref="D59" r:id="rId28" display="https://www.digikey.com/en/products/filter/common-mode-chokes/839?s=N4IgjCBcoEwdIDGUBmBDANgZwKYBoQB7KAbRAGYAOAThhnJAF0CAHAFyhAGU2AnASwB2AcxABfAmGqUooZJHTZ8RUuDjkYANiasOkbnyGiJa6gwTzFuAsUhkYlAOybyjkAU3VNMau5CUAVkoAFjcCalCgvzAABhjNRwhJAMcfJPBNYICAhklM6XSwShhUsPBqMC0Y6LM4bQI4Z1i-OjAAmJgW13JQloDNME0AlsdyMeqGyiHNepAfGOlgnRB2Th4BEXFJWnM5VExrFTtwYJgY4N9JYO8wQtDBsra212ig8hdXkPPogYXLjPIbU6eRyYCWkkoPTM0UolEGMm2VDONUyjgR5XywLmMTA5GoZTgwTx4LmrkcRK6jkc2T6M1uLU0MQCRQZYNxrOCbRG73pzBWegMG2M2xosiQ%2ByUNlU1UYJgAtJ0LFA%2BABXZS2MjDWUEOXwPYKA7q1R43yykyKsiIAAWhAA1jhltoEPwACacXU4vyrfR%2BNgATxYDv0aCwyDEYiAA" xr:uid="{87A834C8-0B7B-4B2F-B104-084480998DC3}"/>
-    <hyperlink ref="D64" r:id="rId29" xr:uid="{841A41E3-9268-4E78-AD7C-2B57CB4E5445}"/>
-    <hyperlink ref="D60" r:id="rId30" xr:uid="{4AD3223F-EADE-48C4-820C-E5411A2E9C66}"/>
-    <hyperlink ref="D65" r:id="rId31" display="https://www.digikey.com/en/products/filter/ceramic-capacitors/60?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbXAFYBOAJlgHYQCxLYAOWeA6gZlbt8YhqANgAMw8hC59h3BgWGVh1SoLij2rNeToqpQ6mHKjqgnv3ogAugQAOAFyggAyvYBOASwB2AcxABfLlFYVWgQZEh0bHwiUgNRAAIAVoAxNWS0pgA6agy1LNg87PIi8CzWUtzUsxzKrLpS7kaspuqCbizKUth60pK2kHIs4VLhYdHy0ros-syQVlqBygLSsESBsCq5uFXZtQaB6nW56i2zA7nuY8FuVsuugfo%2B64UKgdYzplFrmxAHJwAql4PPYAPIoACyODQWAArm4cAECABaCBhCJRXAEYiQMjcSiqAj0LREyiiNTUOjCfabQT8UwEXTkqyBEDI0zoqDuWExHFkcjWfys6lhDwAEycqNE%2Bn%2BkBAgnsAE9bIi5TDkEKgA" xr:uid="{49AC87BF-D071-48BF-BA38-625AFBFBA416}"/>
+    <hyperlink ref="D20" r:id="rId28" xr:uid="{E16FD931-A003-4D30-BCC0-87AABB921E33}"/>
+    <hyperlink ref="D65" r:id="rId29" xr:uid="{F09414C4-69DE-4AFA-8AA8-7F2F7C9358A9}"/>
+    <hyperlink ref="D19" r:id="rId30" xr:uid="{C8DF49F8-E9F7-44BA-8383-3F683F415D56}"/>
+    <hyperlink ref="D62" r:id="rId31" xr:uid="{CB116A6C-D048-4F7B-A387-C71807D4CF96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
almost done digikey -> ozdisan, orange ones are unfinished. red ones are critical
</commit_message>
<xml_diff>
--- a/componentList.xlsx
+++ b/componentList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arda\Documents\ELE713-Two-Switch-Flyback\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arda KASIM\Documents\ELE713-Two-Switch-Flyback\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C84AA1C-887C-4BFC-B7D0-DE0963EDFDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB00DBEF-D7F6-4667-93BB-1AEAEBE8435E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E213F54F-53EC-4B42-AEC9-6F6BEC0714C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E213F54F-53EC-4B42-AEC9-6F6BEC0714C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
   <si>
     <t>Part Number</t>
   </si>
@@ -80,12 +80,6 @@
     <t>Cap: 4.7 µF VDC: 100 V 1210 (DC-link)</t>
   </si>
   <si>
-    <t>SDT5H100LP5-7</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/SDT5H100LP5-7/6702172</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -98,213 +92,21 @@
     <t>CPF0805B100KE</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CPF0805B10KE/2389790</t>
-  </si>
-  <si>
-    <t>Res: 10 kΩ 1/8 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>CPF0805B10KE</t>
-  </si>
-  <si>
-    <t>CL21A475KAQNNNE</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A475KAQNNNE/3886902</t>
-  </si>
-  <si>
-    <t>Cap: 4.7 uF VDC: 25 V 0805</t>
-  </si>
-  <si>
-    <t>PMBT2907A-QR</t>
-  </si>
-  <si>
     <t>PNP</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/PMBT2907A-QR/18634502</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/PMBT2222A-QR/18634518</t>
-  </si>
-  <si>
     <t>NPN</t>
   </si>
   <si>
-    <t>PMBT2222A-QR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/C0805C682K5RAC7800/411156</t>
-  </si>
-  <si>
-    <t>C0805C682K5RAC7800</t>
-  </si>
-  <si>
-    <t>Cap: 6.8 nF VDC: 50 V 0805</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/C0805C103K5RACTU/411157</t>
-  </si>
-  <si>
-    <t>Cap: 10 nF VDC: 50 V 0805</t>
-  </si>
-  <si>
-    <t>C0805C103K5RACTU</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CPF0805B1M1E1/2731308</t>
-  </si>
-  <si>
-    <t>Res: 1.1 MΩ 1/10 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>CPF0805B1M1E1</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CPF-A-0805B12KE/5583862</t>
-  </si>
-  <si>
-    <t>Res: 12 kΩ 1/10 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>CPF-A-0805B12KE</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/C0805C471K5RAC7800/411141</t>
-  </si>
-  <si>
-    <t>Cap: 470 pF VDC: 50 V 0805</t>
-  </si>
-  <si>
-    <t>C0805C471K5RAC7800</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/C0805C101J5GAC7800/411121</t>
-  </si>
-  <si>
-    <t>Cap: 100 pF VDC: 50 V 0805</t>
-  </si>
-  <si>
-    <t>C0805C101J5GAC7800</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/C0805C105K3RAC7210/12701357</t>
-  </si>
-  <si>
-    <t>C0805C105K3RAC7210</t>
-  </si>
-  <si>
-    <t>Cap: 1 uF VDC: 25 V 0805</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/6-2176092-8/4034067</t>
-  </si>
-  <si>
-    <t>6-2176092-8</t>
-  </si>
-  <si>
-    <t>Res: 3.83 kΩ 1/4 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/2-2176093-4/4034128</t>
-  </si>
-  <si>
-    <t>2-2176093-4</t>
-  </si>
-  <si>
-    <t>Res: 16.5 kΩ 1/4 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CPF0805B4K99E1/2383373</t>
-  </si>
-  <si>
-    <t>CPF0805B4K99E1</t>
-  </si>
-  <si>
-    <t>Res: 4.99 kΩ 1/10 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CPF0805B1K0E/2390399</t>
-  </si>
-  <si>
-    <t>CPF0805B1K0E</t>
-  </si>
-  <si>
-    <t>Res: 1 kΩ 1/10 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CPF-A-0805B680RE/5583918</t>
-  </si>
-  <si>
-    <t>CPF-A-0805B680RE</t>
-  </si>
-  <si>
-    <t>Res: 680 Ω 1/10 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CPF-A-0805B39KE/5583901</t>
-  </si>
-  <si>
-    <t>CPF-A-0805B39KE</t>
-  </si>
-  <si>
-    <t>Res: 39 kΩ 1/10 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/2176093-3/4034105</t>
-  </si>
-  <si>
     <t>2176093-3</t>
   </si>
   <si>
-    <t>Res: 9.53 kΩ 1/10 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/5-2176092-1/4034049</t>
-  </si>
-  <si>
-    <t>5-2176092-1</t>
-  </si>
-  <si>
-    <t>Res: 2.49 kΩ 1/10 W 0805 0.1%</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/BZX84-A10-215/2119643</t>
-  </si>
-  <si>
-    <t>ZENER 10V 250 mW</t>
-  </si>
-  <si>
-    <t>BZX84-A10,215</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/TL431LIBQDBZR/9861503</t>
-  </si>
-  <si>
     <t>TL431</t>
   </si>
   <si>
-    <t>TL431LIBQDBZR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/UCC28C55DGKR/18111331</t>
-  </si>
-  <si>
-    <t>UCC28C55DGKR</t>
-  </si>
-  <si>
     <t>Main Controller</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/TLRP3A30CR004FTE/14652341</t>
-  </si>
-  <si>
-    <t>TLRP3A30CR004FTE</t>
-  </si>
-  <si>
-    <t>Res: 4 mΩ 3 W 2512 (Shunt)</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/texas-instruments/ISOM8110DFGR/22119473</t>
   </si>
   <si>
@@ -314,24 +116,12 @@
     <t>Optocoupler</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/vishay-general-semiconductor-diodes-division/V35PWL63-M3-I/16683171</t>
-  </si>
-  <si>
     <t>Secondary Diode</t>
   </si>
   <si>
-    <t>V35PWL63-M3/I</t>
-  </si>
-  <si>
     <t>Primary Diodes</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/infineon-technologies/BSC096N10LS5ATMA1/11500405</t>
-  </si>
-  <si>
-    <t>BSC096N10LS5ATMA1</t>
-  </si>
-  <si>
     <t>Primary MOSFETs</t>
   </si>
   <si>
@@ -410,9 +200,6 @@
     <t>LM5576MHX/NOPB</t>
   </si>
   <si>
-    <t xml:space="preserve">Cap: 1 µF VDC: 100 V 1206  </t>
-  </si>
-  <si>
     <t>https://ozdisan.com/entegre-devreler-icler/guc-entegreleri/dc-dc-voltaj-regulatorleri/LM5576MHXNOPB/585271</t>
   </si>
   <si>
@@ -482,9 +269,6 @@
     <t>https://ozdisan.com/pasif-komponentler/kapasitorler/aluminyum-kapasitorler/EEE-FT1H470AP/1044577</t>
   </si>
   <si>
-    <t xml:space="preserve">Cap Al: 47 µF VDC: 50 V 6.3x5.8  </t>
-  </si>
-  <si>
     <t>https://ozdisan.com/pasif-komponentler/direncler/smt-smd-ve-cip-direncler/1206S4F1021T5E/505049</t>
   </si>
   <si>
@@ -537,19 +321,248 @@
   </si>
   <si>
     <t xml:space="preserve">Schottky VRRM: 100 V Io: 35 A  </t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/1206S4F4221T5E/505095</t>
+  </si>
+  <si>
+    <t>1206S4F4221T5E</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/1206S4F1822T5E/505141</t>
+  </si>
+  <si>
+    <t>1206S4F1822T5E</t>
+  </si>
+  <si>
+    <t>CL31B152KBCNNNC</t>
+  </si>
+  <si>
+    <t>Cap: 1.5 nF VDC: 50 V 1206 (CT)</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/smt-smd-and-mlcc-capacitors/CL31B152KBCNNNC/5693</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/1206S4F5761T5E/505106</t>
+  </si>
+  <si>
+    <t>1206S4F5761T5E</t>
+  </si>
+  <si>
+    <t>Res: 5.76 kΩ 1/4 W 1206 1% (RT)</t>
+  </si>
+  <si>
+    <t>Res: 18.2 kΩ 1/4 W 1206 1% (Rp)</t>
+  </si>
+  <si>
+    <t>Res: 4.22 kΩ 1/4 W 1206 1% (Rcsf)</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/smt-smd-and-mlcc-capacitors/CC1206JRNPO9BN101/750845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC1206JRNPO9BN101 </t>
+  </si>
+  <si>
+    <t>Cap: 100 pF VDC: 50 V 1206</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/smt-smd-and-mlcc-capacitors/CC1206KRX7R9BB682/750181</t>
+  </si>
+  <si>
+    <t>CC1206KRX7R9BB682</t>
+  </si>
+  <si>
+    <t>Cap: 6.8 nF VDC: 50 V 1206</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/smt-smd-and-mlcc-capacitors/C1206C103K5RACTU/704136</t>
+  </si>
+  <si>
+    <t>Cap: 10 nF VDC: 50 V 1206</t>
+  </si>
+  <si>
+    <t>C1206C103K5RACTU</t>
+  </si>
+  <si>
+    <t>CL31B105KBHNNNE</t>
+  </si>
+  <si>
+    <t>Cap: 1 uF VDC: 50 V 1206</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/smt-smd-and-mlcc-capacitors/CL31B105KBHNNNE/15253</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/smt-smd-and-mlcc-capacitors/CL31B475KBHNNNE/369460</t>
+  </si>
+  <si>
+    <t>CL31B475KBHNNNE</t>
+  </si>
+  <si>
+    <t>Cap: 4.7 uF VDC: 50 V 1206</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/precision-power-and-shunt-resistors/BVT-I-R004-1-0/536254</t>
+  </si>
+  <si>
+    <t>BVT-I-R004-1.0</t>
+  </si>
+  <si>
+    <t>Res: 4 mΩ 6 W 2512 (Shunt)</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/1206S4F6800T5E/345241</t>
+  </si>
+  <si>
+    <t>1206S4F6800T5E</t>
+  </si>
+  <si>
+    <t>Res: 680 Ω 1/4 W 1206 1%</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/1206S4F1001T5E/31106</t>
+  </si>
+  <si>
+    <t>Res: 1 kΩ 1/4 W 1206 1%</t>
+  </si>
+  <si>
+    <t>1206S4F1001T5E</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/1206S4F2491T5E/505079</t>
+  </si>
+  <si>
+    <t>Res: 2.49 kΩ 1/4 W 1206 1%</t>
+  </si>
+  <si>
+    <t>1206S4F2491T5E</t>
+  </si>
+  <si>
+    <t>Res: 4.99 kΩ 1/8 W 0805 1%</t>
+  </si>
+  <si>
+    <t>0805S8F4991T5E</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/1206S4F9531T5E/505123</t>
+  </si>
+  <si>
+    <t>Res: 9.53 kΩ 1/4 W 1206 1%</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/CQ06S4F1002T5E/588060</t>
+  </si>
+  <si>
+    <t>Res: 10 kΩ 1/4 W 1206 1%</t>
+  </si>
+  <si>
+    <t>CQ06S4F1002T5E</t>
+  </si>
+  <si>
+    <t>Cap: 1 µF VDC: 100 V 1206  (DC)</t>
+  </si>
+  <si>
+    <t>Cap Al: 47 µF VDC: 50 V 6.3x5.8  (DC)</t>
+  </si>
+  <si>
+    <t>Isolated Supply 12-12</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/1206S4F3902T5E/35634</t>
+  </si>
+  <si>
+    <t>Res: 39 kΩ 1/4 W 1206 1%</t>
+  </si>
+  <si>
+    <t>1206S4F3902T5E</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/smt-smd-and-chip-resistors/0805S8J0115T5E/335350</t>
+  </si>
+  <si>
+    <t>Res: 1.1 MΩ 1/8 W 0805 5%</t>
+  </si>
+  <si>
+    <t>0805S8J0115T5E</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/transistors/discrete-transistors/PZT2222AT1G/476537</t>
+  </si>
+  <si>
+    <t>PZT2222AT1G</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/transistors/discrete-transistors/PZT2907AT1G/476538</t>
+  </si>
+  <si>
+    <t>PZT2907AT1G</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/integrated-circuits-ics/power-management-ics/dc-dc-switching-voltage-controllers/UC3845D8TR/445731</t>
+  </si>
+  <si>
+    <t>UC3845D8TR</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/diodes-diode-modules-and-rectifiers/zener-diodes/BZT585B10T-7/461982</t>
+  </si>
+  <si>
+    <t>BZT585B10T-7</t>
+  </si>
+  <si>
+    <t>ZENER 10V 350 mW</t>
+  </si>
+  <si>
+    <t>TL431LIBQDBZRQ1</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/integrated-circuits-ics/power-management-ics/voltage-reference-ics/TL431LIBQDBZRQ1/1044375</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-supplies/converter-modules/dcdc-converters/R1S-1212-R/539069</t>
+  </si>
+  <si>
+    <t>R1S-1212-R</t>
+  </si>
+  <si>
+    <t>FDD86110</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/mosfets/discrete-mosfets/FDD86110/514788</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/diodes-diode-modules-and-rectifiers/schottky-diodes/V35PWM10HM3I-/743120</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/diodes-diode-modules-and-rectifiers/schottky-diodes/DSSK28-006BS-TRL/642464</t>
+  </si>
+  <si>
+    <t>DSSK28-006BS-TRL</t>
+  </si>
+  <si>
+    <t>V35PWM10HM3/I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -577,7 +590,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,7 +617,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,43 +697,51 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,7 +758,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1047,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248413FF-8C01-4D2A-8D21-504DC00DAF5E}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD54"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,10 +1101,10 @@
         <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>1</v>
@@ -1097,7 +1124,7 @@
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>7</v>
@@ -1109,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -1118,10 +1145,10 @@
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>126</v>
+        <v>55</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -1130,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -1139,10 +1166,10 @@
     </row>
     <row r="4" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>132</v>
+        <v>61</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -1151,7 +1178,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>130</v>
+        <v>59</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
@@ -1160,10 +1187,10 @@
     </row>
     <row r="5" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>135</v>
+        <v>64</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -1172,7 +1199,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
@@ -1181,10 +1208,10 @@
     </row>
     <row r="6" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>137</v>
+        <v>66</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
@@ -1193,7 +1220,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -1202,10 +1229,10 @@
     </row>
     <row r="7" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -1214,7 +1241,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -1223,10 +1250,10 @@
     </row>
     <row r="8" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
@@ -1235,61 +1262,61 @@
         <v>5</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="9">
+    <row r="9" spans="1:9" s="17" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="15">
         <v>3</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="15">
         <v>10</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="9">
+      <c r="E9" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" s="17" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="15">
         <v>2</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="18">
         <v>2</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="E10" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>150</v>
+        <v>78</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -1298,7 +1325,7 @@
         <v>100</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>149</v>
+        <v>77</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -1307,10 +1334,10 @@
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>154</v>
+        <v>82</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>155</v>
+        <v>83</v>
       </c>
       <c r="C12" s="9">
         <v>1</v>
@@ -1319,7 +1346,7 @@
         <v>100</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>153</v>
+        <v>81</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -1328,10 +1355,10 @@
     </row>
     <row r="13" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>157</v>
+        <v>85</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="C13" s="9">
         <v>1</v>
@@ -1340,7 +1367,7 @@
         <v>100</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>156</v>
+        <v>84</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -1349,10 +1376,10 @@
     </row>
     <row r="14" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>161</v>
+        <v>89</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>160</v>
+        <v>88</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
@@ -1361,7 +1388,7 @@
         <v>100</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>159</v>
+        <v>87</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -1370,10 +1397,10 @@
     </row>
     <row r="15" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>165</v>
+        <v>93</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
@@ -1382,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -1390,11 +1417,11 @@
       <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" s="12" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>7447709680</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>163</v>
+        <v>91</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
@@ -1403,580 +1430,688 @@
         <v>1</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="15">
-        <v>1</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="15">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="D21" s="1">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="15">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="15">
-        <v>1</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="15">
-        <v>1</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="15">
-        <v>1</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="15">
-        <v>1</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="15">
-        <v>1</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="15">
-        <v>1</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="15">
-        <v>1</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="15">
-        <v>1</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="15">
-        <v>1</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="15">
-        <v>1</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="15">
-        <v>1</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>32</v>
+      <c r="E22" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>100</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>100</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>100</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>100</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
+      <c r="D31" s="1">
+        <v>100</v>
+      </c>
       <c r="E31" s="2" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>86</v>
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>100</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="C33" s="1">
-        <v>2</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>100</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
+      <c r="D34" s="1">
+        <v>100</v>
+      </c>
       <c r="E34" s="2" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
+      <c r="D35" s="1">
+        <v>100</v>
+      </c>
       <c r="E35" s="2" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>153</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
       <c r="E36" s="2" t="s">
-        <v>44</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
       <c r="E37" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="1">
-        <v>2</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>62</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="17">
+        <v>1</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>158</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
+      <c r="D39" s="1">
+        <v>5</v>
+      </c>
       <c r="E39" s="2" t="s">
-        <v>53</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>57</v>
+        <v>159</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="3">
-        <v>1</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C42" s="3">
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="21">
+        <v>1</v>
+      </c>
+      <c r="D41" s="21">
+        <v>1</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="21">
+        <v>1</v>
+      </c>
+      <c r="D42" s="21">
+        <v>1</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="21">
         <v>2</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="3">
+      <c r="D43" s="21">
         <v>2</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="3">
-        <v>1</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>99</v>
+      <c r="E43" s="22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="21">
+        <v>2</v>
+      </c>
+      <c r="D44" s="21">
+        <v>2</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="C45" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="C46" s="3">
         <v>2</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>105</v>
+      <c r="E46" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C47" s="3">
         <v>2</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>17</v>
+      <c r="E47" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="C48" s="3">
         <v>2</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="C49" s="3">
         <v>2</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>121</v>
+      <c r="E49" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="C50" s="3">
         <v>2</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>108</v>
+      <c r="E50" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C51" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="C52" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>117</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="C53" s="3">
         <v>2</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C55" s="3">
         <v>4</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1" xr:uid="{48F4297B-9724-4DB1-AA26-AC059315FA27}"/>
-    <hyperlink ref="E34" r:id="rId2" xr:uid="{A07D6AF8-5F6C-4482-8C7A-256C06B19C69}"/>
-    <hyperlink ref="E35" r:id="rId3" xr:uid="{DBD7BAD2-9391-4CAC-96FE-2F1937E539ED}"/>
-    <hyperlink ref="E36" r:id="rId4" xr:uid="{FFC0DF21-B008-4D27-8D0F-42E7E0A0F935}"/>
-    <hyperlink ref="E37" r:id="rId5" xr:uid="{9D4F1689-C2DA-49F2-8334-22C073AE08DB}"/>
-    <hyperlink ref="E27" r:id="rId6" xr:uid="{4CE1593A-DBAD-42C8-A00A-A9D074771D62}"/>
-    <hyperlink ref="E39" r:id="rId7" xr:uid="{40D62FDC-CC85-40B0-9F2C-2D24DF52383C}"/>
-    <hyperlink ref="E28" r:id="rId8" xr:uid="{93B4A082-E020-4A96-AC1E-2E1C8BFDE6D2}"/>
-    <hyperlink ref="E23" r:id="rId9" xr:uid="{EE5A321D-E74A-49F1-8794-25FA67083456}"/>
-    <hyperlink ref="E31" r:id="rId10" xr:uid="{1F71484E-12D3-45C1-8C1C-15F79678AC11}"/>
-    <hyperlink ref="E29" r:id="rId11" xr:uid="{61AF3ABB-0019-4725-9847-C34A645E36BF}"/>
-    <hyperlink ref="E44" r:id="rId12" xr:uid="{DBDB070C-5F00-4B1D-B79E-B22511F9D705}"/>
-    <hyperlink ref="E43" r:id="rId13" xr:uid="{01064A09-8CB3-442D-B318-5B154C0B8304}"/>
-    <hyperlink ref="E45" r:id="rId14" xr:uid="{696FF0EA-0FE5-42FF-90DE-163CFC428437}"/>
-    <hyperlink ref="E47" r:id="rId15" xr:uid="{0D6516E8-7CC1-4663-87D0-C1E538F2B339}"/>
-    <hyperlink ref="E54" r:id="rId16" xr:uid="{F09414C4-69DE-4AFA-8AA8-7F2F7C9358A9}"/>
-    <hyperlink ref="E51" r:id="rId17" xr:uid="{CB116A6C-D048-4F7B-A387-C71807D4CF96}"/>
-    <hyperlink ref="E2" r:id="rId18" xr:uid="{FFDC73C4-F386-421A-9E52-D7DE3F4B7142}"/>
-    <hyperlink ref="E3" r:id="rId19" xr:uid="{F50F0C3F-E503-4888-BE01-FE65225214D1}"/>
-    <hyperlink ref="E4" r:id="rId20" xr:uid="{8CE53C47-A47C-4270-9962-6801C95B3EA4}"/>
-    <hyperlink ref="E5" r:id="rId21" xr:uid="{DBE6058D-F39B-4324-9F3B-27457CB11E51}"/>
-    <hyperlink ref="E6" r:id="rId22" xr:uid="{4BDDA0F8-19FC-4467-A07A-418B7CDB4A5E}"/>
-    <hyperlink ref="E7" r:id="rId23" xr:uid="{4A4487C4-22CD-4112-8C8C-129DDCFA4F22}"/>
-    <hyperlink ref="E8" r:id="rId24" xr:uid="{C8E96F8A-EED3-479C-87A6-1C7A915790AA}"/>
-    <hyperlink ref="E9" r:id="rId25" xr:uid="{ADA3DC2C-DAD4-4756-A1A5-B30A70B2F48C}"/>
-    <hyperlink ref="E10" r:id="rId26" xr:uid="{6337422B-04A8-48C3-8A81-2D5BAF095AE1}"/>
-    <hyperlink ref="E11" r:id="rId27" xr:uid="{A8E5D748-CD5A-40F3-845A-A99623422599}"/>
-    <hyperlink ref="E12" r:id="rId28" xr:uid="{1C5B3E7A-BF92-4565-A53D-B637BE89A511}"/>
-    <hyperlink ref="E13" r:id="rId29" xr:uid="{481FB688-EB77-4E6D-86C8-16D0973D0CB3}"/>
-    <hyperlink ref="E14" r:id="rId30" xr:uid="{975D6D5C-908C-4143-AF43-3FA5C1368B70}"/>
-    <hyperlink ref="E16" r:id="rId31" xr:uid="{78D775FF-46BB-42CF-A1A7-409FD3ADF008}"/>
-    <hyperlink ref="E41" r:id="rId32" xr:uid="{1DD7C8E4-5A22-404A-A9F7-9BD21111F2BD}"/>
-    <hyperlink ref="E15" r:id="rId33" xr:uid="{4CAE00F2-988E-4EB1-BA34-BCE58D241AC4}"/>
+    <hyperlink ref="E23" r:id="rId1" xr:uid="{48F4297B-9724-4DB1-AA26-AC059315FA27}"/>
+    <hyperlink ref="E35" r:id="rId2" xr:uid="{A07D6AF8-5F6C-4482-8C7A-256C06B19C69}"/>
+    <hyperlink ref="E30" r:id="rId3" xr:uid="{DBD7BAD2-9391-4CAC-96FE-2F1937E539ED}"/>
+    <hyperlink ref="E18" r:id="rId4" xr:uid="{9D4F1689-C2DA-49F2-8334-22C073AE08DB}"/>
+    <hyperlink ref="E22" r:id="rId5" xr:uid="{4CE1593A-DBAD-42C8-A00A-A9D074771D62}"/>
+    <hyperlink ref="E28" r:id="rId6" xr:uid="{40D62FDC-CC85-40B0-9F2C-2D24DF52383C}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{1F71484E-12D3-45C1-8C1C-15F79678AC11}"/>
+    <hyperlink ref="E38" r:id="rId8" xr:uid="{61AF3ABB-0019-4725-9847-C34A645E36BF}"/>
+    <hyperlink ref="E45" r:id="rId9" xr:uid="{DBDB070C-5F00-4B1D-B79E-B22511F9D705}"/>
+    <hyperlink ref="E44" r:id="rId10" xr:uid="{01064A09-8CB3-442D-B318-5B154C0B8304}"/>
+    <hyperlink ref="E46" r:id="rId11" xr:uid="{696FF0EA-0FE5-42FF-90DE-163CFC428437}"/>
+    <hyperlink ref="E48" r:id="rId12" xr:uid="{0D6516E8-7CC1-4663-87D0-C1E538F2B339}"/>
+    <hyperlink ref="E55" r:id="rId13" xr:uid="{F09414C4-69DE-4AFA-8AA8-7F2F7C9358A9}"/>
+    <hyperlink ref="E52" r:id="rId14" xr:uid="{CB116A6C-D048-4F7B-A387-C71807D4CF96}"/>
+    <hyperlink ref="E2" r:id="rId15" xr:uid="{FFDC73C4-F386-421A-9E52-D7DE3F4B7142}"/>
+    <hyperlink ref="E3" r:id="rId16" xr:uid="{F50F0C3F-E503-4888-BE01-FE65225214D1}"/>
+    <hyperlink ref="E4" r:id="rId17" xr:uid="{8CE53C47-A47C-4270-9962-6801C95B3EA4}"/>
+    <hyperlink ref="E5" r:id="rId18" xr:uid="{DBE6058D-F39B-4324-9F3B-27457CB11E51}"/>
+    <hyperlink ref="E6" r:id="rId19" xr:uid="{4BDDA0F8-19FC-4467-A07A-418B7CDB4A5E}"/>
+    <hyperlink ref="E7" r:id="rId20" xr:uid="{4A4487C4-22CD-4112-8C8C-129DDCFA4F22}"/>
+    <hyperlink ref="E8" r:id="rId21" xr:uid="{C8E96F8A-EED3-479C-87A6-1C7A915790AA}"/>
+    <hyperlink ref="E9" r:id="rId22" xr:uid="{ADA3DC2C-DAD4-4756-A1A5-B30A70B2F48C}"/>
+    <hyperlink ref="E10" r:id="rId23" xr:uid="{6337422B-04A8-48C3-8A81-2D5BAF095AE1}"/>
+    <hyperlink ref="E11" r:id="rId24" xr:uid="{A8E5D748-CD5A-40F3-845A-A99623422599}"/>
+    <hyperlink ref="E12" r:id="rId25" xr:uid="{1C5B3E7A-BF92-4565-A53D-B637BE89A511}"/>
+    <hyperlink ref="E13" r:id="rId26" xr:uid="{481FB688-EB77-4E6D-86C8-16D0973D0CB3}"/>
+    <hyperlink ref="E14" r:id="rId27" xr:uid="{975D6D5C-908C-4143-AF43-3FA5C1368B70}"/>
+    <hyperlink ref="E16" r:id="rId28" xr:uid="{78D775FF-46BB-42CF-A1A7-409FD3ADF008}"/>
+    <hyperlink ref="E42" r:id="rId29" xr:uid="{1DD7C8E4-5A22-404A-A9F7-9BD21111F2BD}"/>
+    <hyperlink ref="E15" r:id="rId30" xr:uid="{4CAE00F2-988E-4EB1-BA34-BCE58D241AC4}"/>
+    <hyperlink ref="E33" r:id="rId31" xr:uid="{5BEF85A2-B24C-48C6-8C6E-A3C3F49C077E}"/>
+    <hyperlink ref="E19" r:id="rId32" xr:uid="{78B280B6-DF94-4AE4-9200-3EF2D5950AD9}"/>
+    <hyperlink ref="E20" r:id="rId33" xr:uid="{CDCBA45F-E22A-4C8B-B0D8-1284792089BF}"/>
+    <hyperlink ref="E21" r:id="rId34" xr:uid="{E04AD5A6-3A60-4AE1-8C5A-528A3E549D2E}"/>
+    <hyperlink ref="E24" r:id="rId35" xr:uid="{23CE448F-782B-4E0D-B4D6-8AA38327332B}"/>
+    <hyperlink ref="E25" r:id="rId36" xr:uid="{6C2E4427-0FF8-41D9-A5FC-7F472FD1C813}"/>
+    <hyperlink ref="E26" r:id="rId37" xr:uid="{12A0AE21-FDA9-44A8-9B25-DC390F58B61B}"/>
+    <hyperlink ref="E27" r:id="rId38" xr:uid="{3FC1DEC6-B008-473F-A9CB-A98FAE84C8BD}"/>
+    <hyperlink ref="E32" r:id="rId39" xr:uid="{7867E9B2-B7AB-4E0D-8E91-A24DDA3468EE}"/>
+    <hyperlink ref="E34" r:id="rId40" xr:uid="{9610D68D-52C1-481A-A64F-DFB6B239A46C}"/>
+    <hyperlink ref="E36" r:id="rId41" xr:uid="{6BFF8417-E1A1-4D75-BD44-F3DB151BE8E3}"/>
+    <hyperlink ref="E37" r:id="rId42" xr:uid="{4117692E-2EDE-4287-94D7-7D9A96950838}"/>
+    <hyperlink ref="E39" r:id="rId43" xr:uid="{CE67D1F6-A003-4CA9-B243-99A2C5675A69}"/>
+    <hyperlink ref="E40" r:id="rId44" xr:uid="{0BFCF954-741E-47DF-9DD6-D86AA0A6A972}"/>
+    <hyperlink ref="E41" r:id="rId45" xr:uid="{46513047-723A-4203-B82B-4318FFF5F2ED}"/>
+    <hyperlink ref="E43" r:id="rId46" xr:uid="{C07BA313-81F5-485F-B08A-58E3C5607758}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>